<commit_message>
Add import button in articles
</commit_message>
<xml_diff>
--- a/src/assets/Contact_Import_Template.xlsx
+++ b/src/assets/Contact_Import_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Invoice India Buhl\invoiz-india-app-react\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Groflex\Repositories\Old groflex repos\groflex-india-app-react\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB202673-3D7D-47D2-B364-369B9C0024D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96994D8-0F0D-4E26-8EDA-A0DF03455C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imprezz Contact Import" sheetId="1" r:id="rId1"/>
@@ -149,28 +149,6 @@
     <t>Discount</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="7.5"/>
-        <color rgb="FFFF3838"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Mandatory field.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Type of customer - possible values: private or company</t>
-    </r>
-  </si>
-  <si>
     <t>GST number of the company (for companies)</t>
   </si>
   <si>
@@ -510,6 +488,21 @@
   </si>
   <si>
     <t>Puducherry</t>
+  </si>
+  <si>
+    <r>
+      <t>Mandatory field.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Type of customer - possible values: Payee or Customer</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -885,43 +878,43 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="15" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="16" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="18" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="20" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="21" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="24" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="15" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1326,33 +1319,33 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="11" width="11.42578125"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="46.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="16" max="17" width="11.42578125"/>
-    <col min="18" max="18" width="10.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" customWidth="1"/>
-    <col min="26" max="1023" width="11.42578125"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="6" width="11.44140625"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="11" width="11.44140625"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="13" max="13" width="46.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" customWidth="1"/>
+    <col min="16" max="17" width="11.44140625"/>
+    <col min="18" max="18" width="10.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" customWidth="1"/>
+    <col min="21" max="21" width="20.44140625" customWidth="1"/>
+    <col min="22" max="22" width="15.88671875" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" customWidth="1"/>
+    <col min="26" max="1023" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1372,7 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
     </row>
-    <row r="2" spans="1:23" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -1414,7 +1407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" ht="39.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="3" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1452,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>17</v>
@@ -1479,145 +1472,145 @@
         <v>24</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="87.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="O4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="V4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:23" s="9" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="9" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="B5" s="7">
         <v>100101</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="R5" s="8"/>
       <c r="S5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="U5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="V5" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="W5" s="7">
         <v>5</v>
@@ -1674,189 +1667,189 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>